<commit_message>
Actualizacion de base de datos del proyecto
Se incluye pk para el usuario creando otra columna para el
nombre_usuario  poligran de cada uno. Tambien se añade tabla INFO donde
hay infomacion basica acerca de la base de datos. Se actualizan archivos
de .DIA .SQL y .XLSX de contenido de la DB
</commit_message>
<xml_diff>
--- a/Db/ESQUEMA BASE DATOS.xlsx
+++ b/Db/ESQUEMA BASE DATOS.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acmartinez2\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktulu\OneDrive - Fundacion Universitaria Politecnico Grancolombiano\1. Administracion de sistemas\6. Semestre\Practica aplicada\ProyectoGitHub\practicaaplicada20172\Db\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entidades" sheetId="1" r:id="rId1"/>
@@ -29,12 +29,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>GUALTEROS GUALTERO DAVID EDUARDO</author>
   </authors>
   <commentList>
-    <comment ref="A68" authorId="0" shapeId="0">
+    <comment ref="A63" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -55,12 +55,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>GUALTEROS GUALTERO DAVID EDUARDO</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -74,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="172">
   <si>
     <t>USUARIO</t>
   </si>
@@ -114,9 +114,6 @@
     <t>pk</t>
   </si>
   <si>
-    <t>llave primaria que identifica a todos los tipos de usuarios, sera el mismo del poligran</t>
-  </si>
-  <si>
     <t>nombre1</t>
   </si>
   <si>
@@ -192,9 +189,6 @@
     <t>tipo_usuario</t>
   </si>
   <si>
-    <t>number</t>
-  </si>
-  <si>
     <t>llave foranea que almacena el id de la el tipo de usuario extraido de la tabla TIPOS_USUARIOS</t>
   </si>
   <si>
@@ -297,9 +291,6 @@
     <t>cupos</t>
   </si>
   <si>
-    <t>number(3)</t>
-  </si>
-  <si>
     <t xml:space="preserve">numero que indica la camtidad maxima de asistentes posibles al evento en caso de que el evento tenga cupos limitados de asistencia </t>
   </si>
   <si>
@@ -456,9 +447,6 @@
     <t>tabla que almacena el registro de logueos de los usuarios, tabla aislada</t>
   </si>
   <si>
-    <t>id_logs</t>
-  </si>
-  <si>
     <t>llave primaria consecutiva que almacena los logs de los usuarios</t>
   </si>
   <si>
@@ -558,35 +546,77 @@
     <t>Cancelar evento</t>
   </si>
   <si>
-    <t>id_favorito</t>
-  </si>
-  <si>
-    <t>favoritos</t>
-  </si>
-  <si>
-    <t>Llave foranea que enlaza a la tabla de favoritos del usuario</t>
-  </si>
-  <si>
-    <t>FAVORITO</t>
-  </si>
-  <si>
-    <t>Tabla donde se almacenan los eventos marcados como favoritos</t>
-  </si>
-  <si>
-    <t>llave primaria que identifica cada favorito</t>
-  </si>
-  <si>
-    <t>llave foranea que identifica el usuario asociado al evento favorito</t>
-  </si>
-  <si>
-    <t>llave foranea que identifica el evento asociado</t>
+    <t>nombre de usuario (el mismo del politecnico grancolombiano)</t>
+  </si>
+  <si>
+    <t>id de usuario unico para cada usuario</t>
+  </si>
+  <si>
+    <t>usuario de poligran</t>
+  </si>
+  <si>
+    <t>smallint</t>
+  </si>
+  <si>
+    <t>smallint(3)</t>
+  </si>
+  <si>
+    <t>id_log</t>
+  </si>
+  <si>
+    <t>varchar(25)</t>
+  </si>
+  <si>
+    <t>nombre de usuario de poligran</t>
+  </si>
+  <si>
+    <t>nombre_usuario</t>
+  </si>
+  <si>
+    <t>INFO</t>
+  </si>
+  <si>
+    <t>id_info</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>decimal(3,1)</t>
+  </si>
+  <si>
+    <t>last_modify</t>
+  </si>
+  <si>
+    <t>about</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>Tabla que contiene informacion sobre la BD</t>
+  </si>
+  <si>
+    <t>llave primaria que muestra las diferentes informaciones</t>
+  </si>
+  <si>
+    <t>numero de version de la BD</t>
+  </si>
+  <si>
+    <t>informacion acerca de la base de datos</t>
+  </si>
+  <si>
+    <t>fecha de modificacion de la version ( 1900-01-01)</t>
+  </si>
+  <si>
+    <t>AUTO_INCREMENT not null</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,6 +628,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -641,6 +685,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -651,13 +701,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF9BBB59"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -772,7 +822,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -793,74 +843,94 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -895,18 +965,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:D24" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:D24" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D24" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="Nº" dataDxfId="3"/>
-    <tableColumn id="2" name="TAREA" dataDxfId="2"/>
-    <tableColumn id="4" name="Prioridad" dataDxfId="1"/>
-    <tableColumn id="3" name="Porcentaje realizado" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nº" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="TAREA" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Prioridad" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Porcentaje realizado" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1208,11 +1278,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:D16"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="8.25" x14ac:dyDescent="0.15"/>
@@ -1226,38 +1296,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="10"/>
       <c r="M1" s="8"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="B2" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>6</v>
-      </c>
+      <c r="E2" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="K2" s="46"/>
+      <c r="M2" s="47"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="11" t="s">
-        <v>7</v>
+        <v>110</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>3</v>
@@ -1267,186 +1339,186 @@
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="12" t="s">
-        <v>8</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" s="11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="11" t="s">
+        <v>4</v>
+      </c>
       <c r="D4" s="11"/>
       <c r="E4" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" s="11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>4</v>
-      </c>
+      <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
-      <c r="I5" s="14"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6" s="11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="11" t="s">
+        <v>4</v>
+      </c>
       <c r="D6" s="11"/>
       <c r="E6" s="12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
+      <c r="I6" s="14"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>4</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
+        <v>13</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="12" t="s">
-        <v>20</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10" s="11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="D10" s="11"/>
       <c r="E10" s="12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11" s="11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="9" t="s">
-        <v>30</v>
+      <c r="D11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>33</v>
+      <c r="D12" s="11"/>
+      <c r="E12" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B13" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A14" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A14" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="B14" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39" t="s">
-        <v>26</v>
-      </c>
+      <c r="B14" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="14" t="s">
-        <v>156</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.15">
@@ -1455,66 +1527,52 @@
       <c r="C15" s="13"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A16" s="43" t="s">
-        <v>157</v>
-      </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
+      <c r="A16" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
       <c r="E16" s="8" t="s">
-        <v>158</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="45" t="s">
-        <v>154</v>
-      </c>
-      <c r="B17" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="45" t="s">
+      <c r="A17" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>159</v>
+      <c r="E17" s="12" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>161</v>
+      <c r="A18" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="16"/>
+      <c r="E18" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>160</v>
-      </c>
+      <c r="A19" s="14"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="14"/>
@@ -1522,263 +1580,281 @@
       <c r="C20" s="13"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="32" t="s">
-        <v>36</v>
+      <c r="A21" s="31" t="s">
+        <v>40</v>
       </c>
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="8" t="s">
-        <v>37</v>
+      <c r="D21" s="33"/>
+      <c r="E21" s="17" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="17" t="s">
+      <c r="A22" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="17"/>
+      <c r="A23" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="11"/>
       <c r="E23" s="12" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="14"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
+      <c r="A24" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="14" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="14"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
+      <c r="A25" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="9" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="18" t="s">
-        <v>43</v>
+      <c r="A26" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="11"/>
+      <c r="E26" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="11" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>45</v>
+      <c r="D27" s="11"/>
+      <c r="E27" s="9" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="11" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="12" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="11" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>50</v>
+        <v>153</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="14" t="s">
-        <v>51</v>
+      <c r="D29" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="11" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>4</v>
+      </c>
       <c r="D30" s="11"/>
-      <c r="E30" s="9" t="s">
-        <v>53</v>
+      <c r="E30" s="18" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="11" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>4</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="C31" s="11"/>
       <c r="D31" s="11"/>
-      <c r="E31" s="9" t="s">
-        <v>56</v>
+      <c r="E31" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="11" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D32" s="11"/>
-      <c r="E32" s="9" t="s">
-        <v>59</v>
+      <c r="E32" s="18" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A33" s="11" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>3</v>
+        <v>153</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="12" t="s">
-        <v>61</v>
+      <c r="D33" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A34" s="11" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>63</v>
+        <v>72</v>
+      </c>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="18" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A35" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="16" t="s">
-        <v>65</v>
-      </c>
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="14"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A36" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="16" t="s">
-        <v>68</v>
-      </c>
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="14"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A37" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="16" t="s">
-        <v>71</v>
+      <c r="A37" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="19" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A38" s="11" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>32</v>
+        <v>153</v>
       </c>
       <c r="C38" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>73</v>
-      </c>
+      <c r="D38" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="F38" s="37"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="37"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A39" s="11" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="16" t="s">
-        <v>76</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="36"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="37"/>
+      <c r="M39" s="37"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A40" s="14"/>
@@ -1789,573 +1865,608 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="14"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A42" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="19" t="s">
-        <v>78</v>
+      <c r="A42" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="34"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="8" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A43" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D43" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="E43" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
-      <c r="K43" s="35"/>
-      <c r="L43" s="35"/>
-      <c r="M43" s="35"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A44" s="11" t="s">
+      <c r="A43" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="B44" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" s="34"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="35"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
-      <c r="K44" s="35"/>
-      <c r="L44" s="35"/>
-      <c r="M44" s="35"/>
+      <c r="B43" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="C43" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="F43" s="40"/>
+      <c r="G43" s="40"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
+      <c r="K43" s="40"/>
+    </row>
+    <row r="44" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="C44" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="39"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="40"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
+      <c r="K44" s="40"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A45" s="14"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="14"/>
+      <c r="A45" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="C45" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="39"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
+      <c r="K45" s="40"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A46" s="14"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
+      <c r="A46" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="9" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A47" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="B47" s="32"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="8" t="s">
-        <v>84</v>
+      <c r="A47" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="16"/>
+      <c r="E47" s="9" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A48" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D48" s="37" t="s">
+      <c r="A48" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="21"/>
+      <c r="E48" s="22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A49" s="23"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="23"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A50" s="14"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A51" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B51" s="34"/>
+      <c r="C51" s="34"/>
+      <c r="D51" s="34"/>
+      <c r="E51" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A52" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E48" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="F48" s="38"/>
-      <c r="G48" s="38"/>
-      <c r="H48" s="38"/>
-      <c r="I48" s="38"/>
-      <c r="J48" s="38"/>
-      <c r="K48" s="38"/>
-    </row>
-    <row r="49" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B49" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C49" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D49" s="37"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="38"/>
-      <c r="I49" s="38"/>
-      <c r="J49" s="38"/>
-      <c r="K49" s="38"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A50" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B50" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C50" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" s="37"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="38"/>
-      <c r="H50" s="38"/>
-      <c r="I50" s="38"/>
-      <c r="J50" s="38"/>
-      <c r="K50" s="38"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A51" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C51" s="22"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A52" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B52" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C52" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D52" s="17"/>
-      <c r="E52" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A53" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" s="23"/>
-      <c r="E53" s="24" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A54" s="25"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="25"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A55" s="14"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="13"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A56" s="32" t="s">
+      <c r="E52" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B56" s="32"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="8" t="s">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A53" s="16" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A57" s="17" t="s">
+      <c r="B53" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="16"/>
+      <c r="E53" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B57" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C57" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D57" s="17" t="s">
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A54" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" s="16"/>
+      <c r="E54" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A55" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A56" s="14"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A57" s="14"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="13"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A58" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="B58" s="34"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A59" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E57" s="12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A58" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="B58" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C58" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D58" s="17"/>
-      <c r="E58" s="12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A59" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="B59" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C59" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D59" s="17"/>
       <c r="E59" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A60" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B60" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D60" s="17" t="s">
-        <v>26</v>
-      </c>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A60" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C60" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="16"/>
       <c r="E60" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.15">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A61" s="14"/>
       <c r="B61" s="13"/>
       <c r="C61" s="13"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A62" s="14"/>
-      <c r="B62" s="13"/>
-      <c r="C62" s="13"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A63" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="B63" s="32"/>
-      <c r="C63" s="32"/>
-      <c r="D63" s="32"/>
+    <row r="62" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="63" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="B63" s="30"/>
+      <c r="C63" s="30"/>
+      <c r="D63" s="30"/>
       <c r="E63" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A64" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="B64" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C64" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D64" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C64" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E64" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A65" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B65" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C65" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D65" s="17"/>
-      <c r="E65" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A66" s="14"/>
-      <c r="B66" s="13"/>
-      <c r="C66" s="13"/>
-    </row>
-    <row r="67" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="E64" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" s="45" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="C65" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="E65" s="45" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" s="11"/>
+      <c r="E66" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="F66" s="27"/>
+      <c r="G66" s="27"/>
+      <c r="H66" s="27"/>
+      <c r="I66" s="27"/>
+      <c r="J66" s="27"/>
+    </row>
+    <row r="67" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67" s="11"/>
+      <c r="E67" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="F67" s="27"/>
+      <c r="G67" s="27"/>
+      <c r="H67" s="27"/>
+      <c r="I67" s="27"/>
+      <c r="J67" s="27"/>
+    </row>
     <row r="68" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="B68" s="31"/>
-      <c r="C68" s="31"/>
-      <c r="D68" s="31"/>
-      <c r="E68" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="B69" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C69" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D69" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="E69" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
+      <c r="A68" s="13"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+    </row>
+    <row r="69" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="70" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B70" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C70" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D70" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E70" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="F70" s="29"/>
-      <c r="G70" s="29"/>
-      <c r="H70" s="29"/>
-      <c r="I70" s="29"/>
-      <c r="J70" s="29"/>
+      <c r="A70" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="B70" s="38"/>
+      <c r="C70" s="38"/>
+      <c r="D70" s="38"/>
+      <c r="E70" s="8" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="71" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="11" t="s">
-        <v>115</v>
+        <v>155</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D71" s="11"/>
-      <c r="E71" s="28" t="s">
+      <c r="D71" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E71" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="F71" s="29"/>
-      <c r="G71" s="29"/>
-      <c r="H71" s="29"/>
-      <c r="I71" s="29"/>
-      <c r="J71" s="29"/>
     </row>
     <row r="72" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="13"/>
-      <c r="B72" s="13"/>
-      <c r="C72" s="13"/>
-      <c r="D72" s="13"/>
-    </row>
-    <row r="73" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="74" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="36" t="s">
+      <c r="A72" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C72" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D72" s="11"/>
+      <c r="E72" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" s="45" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A73" s="51" t="s">
+        <v>158</v>
+      </c>
+      <c r="B73" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="C73" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73" s="42"/>
+      <c r="E73" s="52" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" s="28" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A74" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B74" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C74" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74" s="11"/>
+      <c r="E74" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B74" s="36"/>
-      <c r="C74" s="36"/>
-      <c r="D74" s="36"/>
-      <c r="E74" s="8" t="s">
+    </row>
+    <row r="75" spans="1:10" s="28" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A75" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B75" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="11" t="s">
+      <c r="C75" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D75" s="11"/>
+      <c r="E75" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="B75" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D75" s="11" t="s">
+    </row>
+    <row r="76" spans="1:10" s="28" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A76" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B76" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76" s="11"/>
+      <c r="E76" s="28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A77" s="28"/>
+      <c r="B77" s="28"/>
+      <c r="C77" s="28"/>
+      <c r="D77" s="28"/>
+    </row>
+    <row r="78" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A78" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="B78" s="34"/>
+      <c r="C78" s="34"/>
+      <c r="D78" s="34"/>
+      <c r="E78" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A79" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C79" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D79" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E75" s="9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B76" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C76" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D76" s="11"/>
-      <c r="E76" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B77" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C77" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D77" s="11"/>
-      <c r="E77" s="14" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B78" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D78" s="11"/>
-      <c r="E78" s="30" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B79" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C79" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D79" s="11"/>
-      <c r="E79" s="30" t="s">
+      <c r="E79" s="12" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="30"/>
-      <c r="B80" s="30"/>
-      <c r="C80" s="30"/>
-      <c r="D80" s="30"/>
-    </row>
-    <row r="81" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="32" t="s">
+      <c r="A80" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="B81" s="32"/>
-      <c r="C81" s="32"/>
-      <c r="D81" s="32"/>
-      <c r="E81" s="19" t="s">
+      <c r="B80" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C80" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80" s="16"/>
+      <c r="E80" s="12" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="B82" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C82" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D82" s="17" t="s">
+    <row r="81" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="82" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A82" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="B82" s="54"/>
+      <c r="C82" s="54"/>
+      <c r="D82" s="54"/>
+      <c r="E82" s="47" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A83" s="55" t="s">
+        <v>160</v>
+      </c>
+      <c r="B83" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="C83" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="E82" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="B83" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C83" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D83" s="17"/>
-      <c r="E83" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="E83" s="44" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" s="45" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A84" s="55" t="s">
+        <v>161</v>
+      </c>
+      <c r="B84" s="55" t="s">
+        <v>162</v>
+      </c>
+      <c r="C84" s="57" t="s">
+        <v>171</v>
+      </c>
+      <c r="D84" s="56"/>
+      <c r="E84" s="44" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A85" s="55" t="s">
+        <v>163</v>
+      </c>
+      <c r="B85" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C85" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85" s="56"/>
+      <c r="E85" s="44" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A86" s="55" t="s">
+        <v>164</v>
+      </c>
+      <c r="B86" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="C86" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="D86" s="56"/>
+      <c r="E86" s="44" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E87" s="53"/>
+    </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E43:M44"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="E38:M39"/>
+    <mergeCell ref="A78:D78"/>
     <mergeCell ref="A63:D63"/>
-    <mergeCell ref="D48:D50"/>
-    <mergeCell ref="E48:K50"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="D43:D45"/>
+    <mergeCell ref="E43:K45"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A56:D56"/>
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="A42:D42"/>
-    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="A51:D51"/>
     <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="D38:D39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2364,7 +2475,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2382,16 +2493,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2399,10 +2510,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D2" s="5">
         <v>1</v>
@@ -2413,10 +2524,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
@@ -2427,10 +2538,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D4" s="5">
         <v>1</v>
@@ -2441,10 +2552,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
@@ -2455,10 +2566,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
@@ -2469,10 +2580,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D7" s="5">
         <v>1</v>
@@ -2483,10 +2594,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
@@ -2497,10 +2608,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D9" s="5">
         <v>1</v>
@@ -2511,10 +2622,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D10" s="5">
         <v>1</v>
@@ -2525,7 +2636,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2533,7 +2644,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2541,7 +2652,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2549,7 +2660,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2557,7 +2668,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2565,7 +2676,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Actualizacion de tablas de la BD
Se actualiza tablas de EVENTO y EVENTO_USUARIO para poder manejar los
eliminados sin perder registros

 On branch degualteros

 Changes to be committed:
	modified:   Db/BD v2.5.sql
	modified:   Db/ESQUEMA BASE DATOS.xlsx
	modified:   Db/PoblarBDv2.5.sql
</commit_message>
<xml_diff>
--- a/Db/ESQUEMA BASE DATOS.xlsx
+++ b/Db/ESQUEMA BASE DATOS.xlsx
@@ -9,20 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="51195" windowHeight="26745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entidades" sheetId="1" r:id="rId1"/>
-    <sheet name="Tareas pendientes" sheetId="2" r:id="rId2"/>
+    <sheet name="CODIGOS_COLOR" sheetId="3" r:id="rId2"/>
+    <sheet name="Tareas pendientes" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Tareas pendientes'!$D:$D</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Tareas pendientes'!$D:$D</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -34,7 +38,7 @@
     <author>GUALTEROS GUALTERO DAVID EDUARDO</author>
   </authors>
   <commentList>
-    <comment ref="A64" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A69" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -94,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="221">
   <si>
     <t>USUARIO</t>
   </si>
@@ -660,9 +664,6 @@
     <t>id_comentario</t>
   </si>
   <si>
-    <t>comentario</t>
-  </si>
-  <si>
     <t>llave primaria de la tabla , consecutivo que diferencia cada comentario</t>
   </si>
   <si>
@@ -678,47 +679,95 @@
     <t>COMENTARIO</t>
   </si>
   <si>
-    <t>USUARIONOREGISTRADO</t>
-  </si>
-  <si>
-    <t>id_usuarioNoRegistrado</t>
-  </si>
-  <si>
     <t>not null, auto_increment</t>
   </si>
   <si>
     <t>varchar(500)</t>
   </si>
   <si>
-    <t>agregado_evento</t>
-  </si>
-  <si>
-    <t>registrado_usuario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLA QUE REPRESENTA A LOS USUARIOS QUE ASISTIERON AL EVENTO PERO NO SE REGISTRARON </t>
-  </si>
-  <si>
-    <t>llave primaria consecutivos de tabla</t>
-  </si>
-  <si>
-    <t>nombre de usuario no registrado</t>
-  </si>
-  <si>
-    <t>llave foranea del id_evento al que asistio</t>
-  </si>
-  <si>
-    <t>BOOLEANO QUE REPRESENTA SI EL USUARIO YA FUE AGREGADO A LA TABLA DE EVENTO_USUARIO, ES DECIR QUE YA SE MARCO SU ASISTENCIA</t>
-  </si>
-  <si>
-    <t>BOOLEANO QUE REPRESENTA SI EL USUARIO SE ENCUENTRA DENTRO DE LA TABLA DE USUARIOS</t>
+    <t>marca_eliminado</t>
+  </si>
+  <si>
+    <t>default 0</t>
+  </si>
+  <si>
+    <t>fecha_eliminado</t>
+  </si>
+  <si>
+    <t>fecha_creado</t>
+  </si>
+  <si>
+    <t>fecha_editado</t>
+  </si>
+  <si>
+    <t>fecha_programado</t>
+  </si>
+  <si>
+    <t>current_timestamp</t>
+  </si>
+  <si>
+    <t>dato tipo fecha que guarda la fecha de en la que se realizará el evento</t>
+  </si>
+  <si>
+    <t>Booleano que marca la fecha en la que un usuario elimina un evento</t>
+  </si>
+  <si>
+    <t>Fecha en que el evento es marcado como eliminado por el usuario</t>
+  </si>
+  <si>
+    <t>Booleano que marca un evento como eliminado por el admin</t>
+  </si>
+  <si>
+    <t>Fecha en que el evento es marcado como eliminado por el admin</t>
+  </si>
+  <si>
+    <t>Fecha de la ultima edicion del evento por el admin</t>
+  </si>
+  <si>
+    <t>texto</t>
+  </si>
+  <si>
+    <t>marca_evento_eliminado_usuario</t>
+  </si>
+  <si>
+    <t>fecha_evento_eliminado_usuario</t>
+  </si>
+  <si>
+    <t>AMARILLO</t>
+  </si>
+  <si>
+    <t>CAMBIOS NO HECHOS EN NINGUN ARCHIVO</t>
+  </si>
+  <si>
+    <t>AZUL</t>
+  </si>
+  <si>
+    <t>NARANJA</t>
+  </si>
+  <si>
+    <t>CAMBIOS HECHOS SOLO EN CREACION DE BASE</t>
+  </si>
+  <si>
+    <t>CAMBIOS HECHOS EN CREACION DE BASE Y EN POBLAR BASE</t>
+  </si>
+  <si>
+    <t>VERDE</t>
+  </si>
+  <si>
+    <t>CAMBIOS FALTANTES SOLO EN DIAGRAMA ER Y .DIA</t>
+  </si>
+  <si>
+    <t>BLANCO</t>
+  </si>
+  <si>
+    <t>CAMBIOS YA INCLUIDOS EN TODOS LOS ARCHIVOS DE LA BD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -779,19 +828,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="6"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -801,7 +852,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -816,25 +885,25 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -842,7 +911,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -851,40 +920,40 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -892,30 +961,30 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -925,7 +994,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -948,21 +1017,20 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -973,29 +1041,55 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1006,30 +1100,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1378,10 +1455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M110"/>
+  <dimension ref="A1:M121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="315" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1390,21 +1467,21 @@
     <col min="2" max="2" width="12.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="11.42578125" style="9"/>
     <col min="6" max="6" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
       <c r="E1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="50"/>
+      <c r="K1" s="34"/>
       <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -1423,8 +1500,8 @@
       <c r="E2" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="K2" s="51"/>
-      <c r="M2" s="52"/>
+      <c r="K2" s="35"/>
+      <c r="M2" s="36"/>
     </row>
     <row r="3" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
@@ -1523,10 +1600,10 @@
       <c r="E8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
     </row>
     <row r="9" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
@@ -1626,12 +1703,12 @@
       <c r="C15" s="16"/>
     </row>
     <row r="16" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
       <c r="E16" s="8" t="s">
         <v>34</v>
       </c>
@@ -1679,13 +1756,13 @@
       <c r="C20" s="16"/>
     </row>
     <row r="21" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="45"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="54" t="s">
+      <c r="B21" s="48"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="38" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1723,1171 +1800,1162 @@
     </row>
     <row r="24" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="14" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>4</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C24" s="14"/>
       <c r="D24" s="14"/>
-      <c r="E24" s="17" t="s">
-        <v>47</v>
+      <c r="E24" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="14"/>
+        <v>158</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>4</v>
+      </c>
       <c r="D25" s="14"/>
       <c r="E25" s="9" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="14" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>158</v>
+        <v>54</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>4</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="9" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>54</v>
+        <v>56</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>4</v>
       </c>
       <c r="D27" s="14"/>
-      <c r="E27" s="9" t="s">
-        <v>55</v>
+      <c r="E27" s="15" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="14" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>3</v>
+        <v>146</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="15" t="s">
-        <v>57</v>
+      <c r="D28" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>146</v>
+        <v>3</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="14" t="s">
-        <v>25</v>
-      </c>
+      <c r="D29" s="14"/>
       <c r="E29" s="19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="14" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>4</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="C30" s="14"/>
       <c r="D30" s="14"/>
       <c r="E30" s="19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="C31" s="14"/>
+        <v>65</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>4</v>
+      </c>
       <c r="D31" s="14"/>
       <c r="E31" s="19" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="14" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>65</v>
+        <v>146</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="14"/>
+      <c r="D32" s="14" t="s">
+        <v>25</v>
+      </c>
       <c r="E32" s="19" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B33" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" s="43" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="41" t="s">
+        <v>200</v>
+      </c>
+      <c r="B34" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="41"/>
+      <c r="E34" s="42" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" s="43" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="41" t="s">
+        <v>198</v>
+      </c>
+      <c r="B35" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="41"/>
+      <c r="E35" s="42" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" s="43" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="B36" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="D36" s="41"/>
+      <c r="E36" s="42" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" s="43" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="44" t="s">
+        <v>197</v>
+      </c>
+      <c r="B37" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="42" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" s="43" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="B38" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="44" t="s">
+        <v>201</v>
+      </c>
+      <c r="D38" s="44"/>
+      <c r="E38" s="42" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="17"/>
+    </row>
+    <row r="40" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="46"/>
+      <c r="C40" s="46"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="C33" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="17"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="17"/>
-    </row>
-    <row r="36" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="17"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="17"/>
-    </row>
-    <row r="37" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="40" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="55" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" s="14" t="s">
+      <c r="C41" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="E41" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="F41" s="53"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="53"/>
+      <c r="J41" s="53"/>
+      <c r="K41" s="53"/>
+      <c r="L41" s="53"/>
+      <c r="M41" s="53"/>
+    </row>
+    <row r="42" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="C38" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="48" t="s">
-        <v>75</v>
-      </c>
-      <c r="E38" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="F38" s="38"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="38"/>
-      <c r="I38" s="38"/>
-      <c r="J38" s="38"/>
-      <c r="K38" s="38"/>
-      <c r="L38" s="38"/>
-      <c r="M38" s="38"/>
-    </row>
-    <row r="39" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="B39" s="14" t="s">
+      <c r="C42" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="52"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="53"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="53"/>
+      <c r="L42" s="53"/>
+      <c r="M42" s="53"/>
+    </row>
+    <row r="43" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="17"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="17"/>
+    </row>
+    <row r="44" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="17"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+    </row>
+    <row r="45" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45" s="50"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="C39" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="48"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="38"/>
-      <c r="I39" s="38"/>
-      <c r="J39" s="38"/>
-      <c r="K39" s="38"/>
-      <c r="L39" s="38"/>
-      <c r="M39" s="38"/>
-    </row>
-    <row r="40" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="17"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="17"/>
-    </row>
-    <row r="41" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="17"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
-    </row>
-    <row r="42" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="47"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B43" s="20" t="s">
+      <c r="C46" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="F46" s="56"/>
+      <c r="G46" s="56"/>
+      <c r="H46" s="56"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="56"/>
+      <c r="K46" s="56"/>
+    </row>
+    <row r="47" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="C43" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D43" s="42" t="s">
+      <c r="C47" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="55"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="56"/>
+      <c r="G47" s="56"/>
+      <c r="H47" s="56"/>
+      <c r="I47" s="56"/>
+      <c r="J47" s="56"/>
+      <c r="K47" s="56"/>
+    </row>
+    <row r="48" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="C48" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="55"/>
+      <c r="E48" s="56"/>
+      <c r="F48" s="56"/>
+      <c r="G48" s="56"/>
+      <c r="H48" s="56"/>
+      <c r="I48" s="56"/>
+      <c r="J48" s="56"/>
+      <c r="K48" s="56"/>
+    </row>
+    <row r="49" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="18"/>
+      <c r="E50" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="21"/>
+      <c r="E51" s="22" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="21"/>
+      <c r="E52" s="23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="43" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="41" t="s">
+        <v>209</v>
+      </c>
+      <c r="B53" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="D53" s="41"/>
+      <c r="E53" s="42" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="43" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="44" t="s">
+        <v>210</v>
+      </c>
+      <c r="B54" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C54" s="44"/>
+      <c r="D54" s="44"/>
+      <c r="E54" s="42" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="17"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="16"/>
+    </row>
+    <row r="56" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="B56" s="48"/>
+      <c r="C56" s="48"/>
+      <c r="D56" s="49"/>
+      <c r="E56" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E43" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
-      <c r="K43" s="43"/>
-    </row>
-    <row r="44" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B44" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="C44" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" s="42"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="43"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
-      <c r="K44" s="43"/>
-    </row>
-    <row r="45" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="C45" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" s="42"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
-      <c r="K45" s="43"/>
-    </row>
-    <row r="46" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="B46" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B47" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C47" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" s="18"/>
-      <c r="E47" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D48" s="22"/>
-      <c r="E48" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D49" s="22"/>
-      <c r="E49" s="24" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="17"/>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16"/>
-    </row>
-    <row r="51" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="B51" s="39"/>
-      <c r="C51" s="39"/>
-      <c r="D51" s="39"/>
-      <c r="E51" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="B52" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="C52" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D52" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E52" s="15" t="s">
+      <c r="E57" s="15" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="18" t="s">
+    <row r="58" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B53" s="11" t="s">
+      <c r="B58" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C53" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" s="18"/>
-      <c r="E53" s="15" t="s">
+      <c r="C58" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" s="18"/>
+      <c r="E58" s="15" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="B54" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C54" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D54" s="18"/>
-      <c r="E54" s="15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="B55" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="C55" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D55" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="17"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16"/>
-    </row>
-    <row r="57" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="17"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="16"/>
-    </row>
-    <row r="58" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="B58" s="39"/>
-      <c r="C58" s="39"/>
-      <c r="D58" s="39"/>
-      <c r="E58" s="8" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="B59" s="14" t="s">
-        <v>146</v>
+        <v>93</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="C59" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D59" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E59" s="34" t="s">
-        <v>99</v>
+      <c r="D59" s="18"/>
+      <c r="E59" s="15" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="B60" s="18" t="s">
-        <v>43</v>
+        <v>98</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>146</v>
       </c>
       <c r="C60" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D60" s="18"/>
-      <c r="E60" s="34" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" s="37" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="B61" s="35" t="s">
-        <v>146</v>
-      </c>
-      <c r="C61" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D61" s="35"/>
-      <c r="E61" s="36" t="s">
-        <v>181</v>
-      </c>
+      <c r="D60" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E60" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="17"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="16"/>
     </row>
     <row r="62" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="17"/>
       <c r="B62" s="16"/>
       <c r="C62" s="16"/>
     </row>
+    <row r="63" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="B63" s="50"/>
+      <c r="C63" s="50"/>
+      <c r="D63" s="50"/>
+      <c r="E63" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
     <row r="64" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="40" t="s">
-        <v>101</v>
-      </c>
-      <c r="B64" s="40"/>
-      <c r="C64" s="40"/>
-      <c r="D64" s="40"/>
-      <c r="E64" s="8" t="s">
-        <v>102</v>
+      <c r="A64" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E64" s="33" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="B65" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="C65" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D65" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>104</v>
+      <c r="A65" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="B65" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" s="18"/>
+      <c r="E65" s="33" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:10" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="12" t="s">
-        <v>2</v>
+      <c r="A66" s="11" t="s">
+        <v>171</v>
       </c>
       <c r="B66" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="C66" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D66" s="27" t="s">
+      <c r="C66" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" s="11"/>
+      <c r="E66" s="29" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="17"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="16"/>
+    </row>
+    <row r="69" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="B69" s="46"/>
+      <c r="C69" s="46"/>
+      <c r="D69" s="46"/>
+      <c r="E69" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A70" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C70" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A71" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C71" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D71" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E66" s="13" t="s">
+      <c r="E71" s="13" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="B67" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C67" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D67" s="14"/>
-      <c r="E67" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="F67" s="29"/>
-      <c r="G67" s="29"/>
-      <c r="H67" s="29"/>
-      <c r="I67" s="29"/>
-      <c r="J67" s="29"/>
-    </row>
-    <row r="68" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="B68" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="C68" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D68" s="14"/>
-      <c r="E68" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="F68" s="29"/>
-      <c r="G68" s="29"/>
-      <c r="H68" s="29"/>
-      <c r="I68" s="29"/>
-      <c r="J68" s="29"/>
-    </row>
-    <row r="69" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="16"/>
-      <c r="B69" s="16"/>
-      <c r="C69" s="16"/>
-      <c r="D69" s="16"/>
-    </row>
-    <row r="71" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="B71" s="41"/>
-      <c r="C71" s="41"/>
-      <c r="D71" s="41"/>
-      <c r="E71" s="8" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="14" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>146</v>
+        <v>3</v>
       </c>
       <c r="C72" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D72" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E72" s="9" t="s">
-        <v>111</v>
-      </c>
+      <c r="D72" s="14"/>
+      <c r="E72" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="F72" s="28"/>
+      <c r="G72" s="28"/>
+      <c r="H72" s="28"/>
+      <c r="I72" s="28"/>
+      <c r="J72" s="28"/>
     </row>
     <row r="73" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73" s="14"/>
+      <c r="E73" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="F73" s="28"/>
+      <c r="G73" s="28"/>
+      <c r="H73" s="28"/>
+      <c r="I73" s="28"/>
+      <c r="J73" s="28"/>
+    </row>
+    <row r="74" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A74" s="16"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="16"/>
+    </row>
+    <row r="76" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A76" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="B76" s="54"/>
+      <c r="C76" s="54"/>
+      <c r="D76" s="54"/>
+      <c r="E76" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A77" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D77" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A78" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B73" s="14" t="s">
+      <c r="B78" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="C73" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D73" s="14"/>
-      <c r="E73" s="15" t="s">
+      <c r="C78" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78" s="14"/>
+      <c r="E78" s="15" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="74" spans="1:10" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="11" t="s">
+    <row r="79" spans="1:10" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A79" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="B74" s="11" t="s">
+      <c r="B79" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="C74" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D74" s="11"/>
-      <c r="E74" s="30" t="s">
+      <c r="C79" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D79" s="11"/>
+      <c r="E79" s="29" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="75" spans="1:10" s="31" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="14" t="s">
+    <row r="80" spans="1:10" s="30" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A80" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B75" s="26" t="s">
+      <c r="B80" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C75" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D75" s="14"/>
-      <c r="E75" s="17" t="s">
+      <c r="C80" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80" s="14"/>
+      <c r="E80" s="17" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="76" spans="1:10" s="31" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="14" t="s">
+    <row r="81" spans="1:5" s="30" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A81" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B76" s="11" t="s">
+      <c r="B81" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C76" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D76" s="14"/>
-      <c r="E76" s="31" t="s">
+      <c r="C81" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81" s="14"/>
+      <c r="E81" s="30" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="77" spans="1:10" s="31" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="14" t="s">
+    <row r="82" spans="1:5" s="30" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A82" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B77" s="11" t="s">
+      <c r="B82" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="C77" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D77" s="14"/>
-      <c r="E77" s="31" t="s">
+      <c r="C82" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" s="14"/>
+      <c r="E82" s="30" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="31"/>
-      <c r="B78" s="31"/>
-      <c r="C78" s="31"/>
-      <c r="D78" s="31"/>
-    </row>
-    <row r="79" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="39" t="s">
+    <row r="83" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A83" s="30"/>
+      <c r="B83" s="30"/>
+      <c r="C83" s="30"/>
+      <c r="D83" s="30"/>
+    </row>
+    <row r="84" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A84" s="50" t="s">
         <v>115</v>
       </c>
-      <c r="B79" s="39"/>
-      <c r="C79" s="39"/>
-      <c r="D79" s="39"/>
-      <c r="E79" s="55" t="s">
+      <c r="B84" s="50"/>
+      <c r="C84" s="50"/>
+      <c r="D84" s="50"/>
+      <c r="E84" s="39" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="18" t="s">
+    <row r="85" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A85" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="B80" s="14" t="s">
+      <c r="B85" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="C80" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D80" s="18" t="s">
+      <c r="C85" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E80" s="15" t="s">
+      <c r="E85" s="15" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="18" t="s">
+    <row r="86" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A86" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="B81" s="11" t="s">
+      <c r="B86" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="C81" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D81" s="18"/>
-      <c r="E81" s="15" t="s">
+      <c r="C86" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D86" s="18"/>
+      <c r="E86" s="15" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="83" spans="1:5" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="49" t="s">
+    <row r="88" spans="1:5" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A88" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="B83" s="49"/>
-      <c r="C83" s="49"/>
-      <c r="D83" s="49"/>
-      <c r="E83" s="52" t="s">
+      <c r="B88" s="45"/>
+      <c r="C88" s="45"/>
+      <c r="D88" s="45"/>
+      <c r="E88" s="36" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="84" spans="1:5" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="32" t="s">
+    <row r="89" spans="1:5" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A89" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="B84" s="32" t="s">
+      <c r="B89" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="C84" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D84" s="32" t="s">
+      <c r="C89" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D89" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E84" s="13" t="s">
+      <c r="E89" s="13" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="32" t="s">
+    <row r="90" spans="1:5" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A90" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="B85" s="32" t="s">
+      <c r="B90" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="C85" s="33" t="s">
+      <c r="C90" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="D85" s="32"/>
-      <c r="E85" s="13" t="s">
+      <c r="D90" s="31"/>
+      <c r="E90" s="13" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="32" t="s">
+    <row r="91" spans="1:5" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A91" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="B86" s="32" t="s">
+      <c r="B91" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C86" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D86" s="32"/>
-      <c r="E86" s="13" t="s">
+      <c r="C91" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D91" s="31"/>
+      <c r="E91" s="13" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="87" spans="1:5" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="32" t="s">
+    <row r="92" spans="1:5" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A92" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="B87" s="32" t="s">
+      <c r="B92" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="C87" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D87" s="32"/>
-      <c r="E87" s="13" t="s">
+      <c r="C92" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D92" s="31"/>
+      <c r="E92" s="13" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="49" t="s">
+    <row r="94" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A94" s="45" t="s">
         <v>167</v>
       </c>
-      <c r="B89" s="49"/>
-      <c r="C89" s="49"/>
-      <c r="D89" s="49"/>
-      <c r="E89" s="8" t="s">
+      <c r="B94" s="45"/>
+      <c r="C94" s="45"/>
+      <c r="D94" s="45"/>
+      <c r="E94" s="8" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A90" s="32" t="s">
+    <row r="95" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A95" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="B90" s="32" t="s">
+      <c r="B95" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="C90" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D90" s="32" t="s">
+      <c r="C95" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D95" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E90" s="9" t="s">
+      <c r="E95" s="9" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="32" t="s">
+    <row r="96" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A96" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="B91" s="32" t="s">
+      <c r="B96" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="C91" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D91" s="32"/>
-      <c r="E91" s="9" t="s">
+      <c r="C96" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D96" s="31"/>
+      <c r="E96" s="9" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="32" t="s">
+    <row r="97" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A97" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="B92" s="32" t="str">
-        <f>B59</f>
+      <c r="B97" s="31" t="str">
+        <f>B64</f>
         <v>smallint</v>
       </c>
-      <c r="C92" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D92" s="32" t="s">
+      <c r="C97" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D97" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E92" s="9" t="s">
+      <c r="E97" s="9" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="32" t="s">
+    <row r="98" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A98" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="B93" s="32" t="str">
-        <f>B52</f>
+      <c r="B98" s="31" t="str">
+        <f>B57</f>
         <v>smallint</v>
       </c>
-      <c r="C93" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D93" s="32" t="s">
+      <c r="C98" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D98" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E93" s="9" t="s">
+      <c r="E98" s="9" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="32" t="s">
+    <row r="99" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A99" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="B94" s="32" t="s">
+      <c r="B99" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="C94" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D94" s="32"/>
-      <c r="E94" s="9" t="s">
+      <c r="C99" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D99" s="31"/>
+      <c r="E99" s="9" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A95" s="32" t="s">
+    <row r="100" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A100" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B95" s="32" t="s">
+      <c r="B100" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="C95" s="32"/>
-      <c r="D95" s="32"/>
-      <c r="E95" s="9" t="s">
+      <c r="C100" s="31"/>
+      <c r="D100" s="31"/>
+      <c r="E100" s="9" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="32" t="s">
+    <row r="101" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A101" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="B96" s="32" t="s">
+      <c r="B101" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="C96" s="32"/>
-      <c r="D96" s="32"/>
-      <c r="E96" s="9" t="s">
+      <c r="C101" s="31"/>
+      <c r="D101" s="31"/>
+      <c r="E101" s="9" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="49" t="s">
+    <row r="103" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A103" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="B103" s="45"/>
+      <c r="C103" s="45"/>
+      <c r="D103" s="45"/>
+      <c r="E103" s="8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A104" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="B104" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="C104" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="B98" s="49"/>
-      <c r="C98" s="49"/>
-      <c r="D98" s="49"/>
-      <c r="E98" s="8" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="32" t="s">
-        <v>187</v>
-      </c>
-      <c r="B99" s="32" t="s">
+      <c r="D104" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E104" s="9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A105" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B105" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="C99" s="32" t="s">
-        <v>196</v>
-      </c>
-      <c r="D99" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="E99" s="9" t="s">
+      <c r="C105" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D105" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E105" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A106" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B106" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="C106" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D106" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E106" s="13" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="B100" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="C100" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D100" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="E100" s="13" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A101" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="B101" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="C101" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D101" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="E101" s="13" t="s">
+    <row r="107" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A107" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B107" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="C107" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D107" s="31"/>
+      <c r="E107" s="9" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="32" t="s">
-        <v>188</v>
-      </c>
-      <c r="B102" s="32" t="s">
-        <v>197</v>
-      </c>
-      <c r="C102" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D102" s="32"/>
-      <c r="E102" s="9" t="s">
+    <row r="108" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A108" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B108" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C108" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D108" s="31"/>
+      <c r="E108" s="9" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="B103" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="C103" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D103" s="32"/>
-      <c r="E103" s="9" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A105" s="49" t="s">
-        <v>194</v>
-      </c>
-      <c r="B105" s="49"/>
-      <c r="C105" s="49"/>
-      <c r="D105" s="49"/>
-      <c r="E105" s="8" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="32" t="s">
-        <v>195</v>
-      </c>
-      <c r="B106" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="C106" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D106" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="E106" s="9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A107" s="32" t="s">
-        <v>151</v>
-      </c>
-      <c r="B107" s="32" t="s">
-        <v>149</v>
-      </c>
-      <c r="C107" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D107" s="32"/>
-      <c r="E107" s="13" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="B108" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="C108" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D108" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="E108" s="13" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A109" s="32" t="s">
-        <v>198</v>
-      </c>
-      <c r="B109" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C109" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D109" s="32"/>
-      <c r="E109" s="9" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A110" s="32" t="s">
-        <v>199</v>
-      </c>
-      <c r="B110" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C110" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D110" s="32"/>
-      <c r="E110" s="9" t="s">
-        <v>205</v>
-      </c>
+    <row r="121" spans="3:3" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C121" s="57"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A98:D98"/>
-    <mergeCell ref="A105:D105"/>
-    <mergeCell ref="A89:D89"/>
+  <mergeCells count="17">
+    <mergeCell ref="E41:M42"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A76:D76"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="D46:D48"/>
+    <mergeCell ref="E46:K48"/>
+    <mergeCell ref="A103:D103"/>
+    <mergeCell ref="A94:D94"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A56:D56"/>
     <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="A83:D83"/>
-    <mergeCell ref="E38:M39"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="D43:D45"/>
-    <mergeCell ref="E43:K45"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="A88:D88"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2896,6 +2964,91 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1725249-2B3F-4F80-87DD-B3AF504730AD}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="A1:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="60" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="61" t="s">
+        <v>213</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="62" t="s">
+        <v>217</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>218</v>
+      </c>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="63" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>220</v>
+      </c>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>

</xml_diff>

<commit_message>
Modificacion de PK en tabla SESION
Se cambia ID_SESION a VARCHAR(50) por mejora en codigo

 Changes to be committed:
	modified:   Db/BD v2.5.sql
	modified:   Db/ESQUEMA BASE DATOS.xlsx
</commit_message>
<xml_diff>
--- a/Db/ESQUEMA BASE DATOS.xlsx
+++ b/Db/ESQUEMA BASE DATOS.xlsx
@@ -782,7 +782,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -844,6 +844,14 @@
     </font>
     <font>
       <b/>
+      <u/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="8"/>
       <color rgb="FF000000"/>
@@ -1009,7 +1017,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1035,10 +1043,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1057,19 +1061,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1077,23 +1069,8 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1111,24 +1088,62 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1479,1628 +1494,1624 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" zoomScalePageLayoutView="315" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" zoomScalePageLayoutView="315" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.42578125" style="16"/>
-    <col min="6" max="6" width="14.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="16"/>
+    <col min="1" max="1" width="19.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.42578125" style="14"/>
+    <col min="6" max="6" width="14.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="M1" s="15"/>
-    </row>
-    <row r="2" spans="1:13" s="21" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+      <c r="K1" s="15"/>
+      <c r="M1" s="13"/>
+    </row>
+    <row r="2" spans="1:13" s="19" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="20" t="s">
+      <c r="C2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="K2" s="22"/>
-      <c r="M2" s="23"/>
+      <c r="K2" s="20"/>
+      <c r="M2" s="21"/>
     </row>
     <row r="3" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25" t="s">
+      <c r="C3" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="23" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25" t="s">
+      <c r="C4" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="25" t="s">
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
     </row>
     <row r="6" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="25" t="s">
+      <c r="C6" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="27"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
     </row>
     <row r="7" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="25" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25" t="s">
+      <c r="C8" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="22"/>
+      <c r="E8" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
     </row>
     <row r="9" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25" t="s">
+      <c r="C9" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="22"/>
+      <c r="E9" s="23" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25" t="s">
+      <c r="C10" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="22"/>
+      <c r="E10" s="23" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="24" t="s">
+      <c r="C11" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="23" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="16" t="s">
+      <c r="C12" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="22"/>
+      <c r="E12" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="C13" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="24" t="s">
+      <c r="C13" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="23" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="27" t="s">
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="25" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="27"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
     </row>
     <row r="16" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="15" t="s">
+      <c r="B16" s="59"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="13" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="C17" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="30" t="s">
+      <c r="C17" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="23" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="25" t="s">
+      <c r="C18" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="27"/>
+      <c r="E18" s="23" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="27"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
     </row>
     <row r="20" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="27"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
     </row>
     <row r="21" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="34" t="s">
+      <c r="B21" s="57"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="28" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="C22" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="24" t="s">
+      <c r="C22" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="23" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="25" t="s">
+      <c r="C23" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="22"/>
+      <c r="E23" s="23" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="16" t="s">
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="14" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="C25" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="24"/>
-      <c r="E25" s="16" t="s">
+      <c r="C25" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="22"/>
+      <c r="E25" s="14" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="24"/>
-      <c r="E26" s="16" t="s">
+      <c r="C26" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="22"/>
+      <c r="E26" s="14" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="C27" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="67" t="s">
+      <c r="C27" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="35" t="s">
+      <c r="E27" s="29" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="C28" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="24" t="s">
+      <c r="C28" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="35" t="s">
+      <c r="E28" s="29" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="24"/>
-      <c r="E29" s="35" t="s">
+      <c r="C29" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="22"/>
+      <c r="E29" s="29" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="35" t="s">
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="29" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="24"/>
-      <c r="E31" s="35" t="s">
+      <c r="C31" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="22"/>
+      <c r="E31" s="29" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="C32" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="24" t="s">
+      <c r="C32" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="35" t="s">
+      <c r="E32" s="29" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="24" t="s">
+      <c r="B33" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="35" t="s">
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="29" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="38" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="36" t="s">
+    <row r="34" spans="1:13" s="32" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="B34" s="36" t="s">
+      <c r="B34" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="36"/>
-      <c r="E34" s="37" t="s">
+      <c r="C34" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="30"/>
+      <c r="E34" s="31" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="38" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="36" t="s">
+    <row r="35" spans="1:13" s="32" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="30" t="s">
         <v>197</v>
       </c>
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="36"/>
-      <c r="E35" s="37" t="s">
+      <c r="C35" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="30"/>
+      <c r="E35" s="31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="38" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="36" t="s">
+    <row r="36" spans="1:13" s="32" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="30" t="s">
         <v>194</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C36" s="36" t="s">
+      <c r="C36" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="D36" s="36"/>
-      <c r="E36" s="37" t="s">
+      <c r="D36" s="30"/>
+      <c r="E36" s="31" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="38" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="39" t="s">
+    <row r="37" spans="1:13" s="32" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="33" t="s">
         <v>196</v>
       </c>
-      <c r="B37" s="39" t="s">
+      <c r="B37" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="39" t="s">
+      <c r="C37" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="D37" s="39"/>
-      <c r="E37" s="37" t="s">
+      <c r="D37" s="33"/>
+      <c r="E37" s="31" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="38" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="39" t="s">
+    <row r="38" spans="1:13" s="32" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="B38" s="39" t="s">
+      <c r="B38" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="C38" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="D38" s="39"/>
-      <c r="E38" s="37" t="s">
+      <c r="D38" s="33"/>
+      <c r="E38" s="31" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="27"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="27"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="25"/>
     </row>
     <row r="40" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="40" t="s">
+      <c r="B40" s="55"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="34" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="24" t="s">
+      <c r="A41" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="24" t="s">
+      <c r="B41" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="C41" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" s="41" t="s">
+      <c r="C41" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="E41" s="42" t="s">
+      <c r="E41" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="42"/>
-      <c r="J41" s="42"/>
-      <c r="K41" s="42"/>
-      <c r="L41" s="42"/>
-      <c r="M41" s="42"/>
+      <c r="F41" s="63"/>
+      <c r="G41" s="63"/>
+      <c r="H41" s="63"/>
+      <c r="I41" s="63"/>
+      <c r="J41" s="63"/>
+      <c r="K41" s="63"/>
+      <c r="L41" s="63"/>
+      <c r="M41" s="63"/>
     </row>
     <row r="42" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="24" t="s">
+      <c r="A42" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B42" s="24" t="s">
+      <c r="B42" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="C42" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" s="41"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="42"/>
-      <c r="J42" s="42"/>
-      <c r="K42" s="42"/>
-      <c r="L42" s="42"/>
-      <c r="M42" s="42"/>
+      <c r="C42" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="61"/>
+      <c r="E42" s="63"/>
+      <c r="F42" s="63"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="63"/>
+      <c r="J42" s="63"/>
+      <c r="K42" s="63"/>
+      <c r="L42" s="63"/>
+      <c r="M42" s="63"/>
     </row>
     <row r="43" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="27"/>
-      <c r="I43" s="43"/>
+      <c r="A43" s="25"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="25"/>
+      <c r="I43" s="35"/>
     </row>
     <row r="44" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="27"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
     </row>
     <row r="45" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="29" t="s">
+      <c r="A45" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="B45" s="29"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="15" t="s">
+      <c r="B45" s="59"/>
+      <c r="C45" s="60"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="13" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="45" t="s">
+      <c r="A46" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="B46" s="45" t="s">
+      <c r="B46" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="C46" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="D46" s="46" t="s">
+      <c r="C46" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="E46" s="47" t="s">
+      <c r="E46" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="F46" s="47"/>
-      <c r="G46" s="47"/>
-      <c r="H46" s="47"/>
-      <c r="I46" s="47"/>
-      <c r="J46" s="47"/>
-      <c r="K46" s="47"/>
+      <c r="F46" s="66"/>
+      <c r="G46" s="66"/>
+      <c r="H46" s="66"/>
+      <c r="I46" s="66"/>
+      <c r="J46" s="66"/>
+      <c r="K46" s="66"/>
     </row>
     <row r="47" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="45" t="s">
+      <c r="A47" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="45" t="s">
+      <c r="B47" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="C47" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" s="46"/>
-      <c r="E47" s="47"/>
-      <c r="F47" s="47"/>
-      <c r="G47" s="47"/>
-      <c r="H47" s="47"/>
-      <c r="I47" s="47"/>
-      <c r="J47" s="47"/>
-      <c r="K47" s="47"/>
+      <c r="C47" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="65"/>
+      <c r="E47" s="66"/>
+      <c r="F47" s="66"/>
+      <c r="G47" s="66"/>
+      <c r="H47" s="66"/>
+      <c r="I47" s="66"/>
+      <c r="J47" s="66"/>
+      <c r="K47" s="66"/>
     </row>
     <row r="48" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="45" t="s">
+      <c r="A48" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="45" t="s">
+      <c r="B48" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="C48" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="D48" s="46"/>
-      <c r="E48" s="47"/>
-      <c r="F48" s="47"/>
-      <c r="G48" s="47"/>
-      <c r="H48" s="47"/>
-      <c r="I48" s="47"/>
-      <c r="J48" s="47"/>
-      <c r="K48" s="47"/>
+      <c r="C48" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="65"/>
+      <c r="E48" s="66"/>
+      <c r="F48" s="66"/>
+      <c r="G48" s="66"/>
+      <c r="H48" s="66"/>
+      <c r="I48" s="66"/>
+      <c r="J48" s="66"/>
+      <c r="K48" s="66"/>
     </row>
     <row r="49" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="30" t="s">
+      <c r="A49" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="B49" s="30" t="s">
+      <c r="B49" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C49" s="48"/>
-      <c r="D49" s="48"/>
-      <c r="E49" s="16" t="s">
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="14" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="24" t="s">
+      <c r="A50" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="B50" s="30" t="s">
+      <c r="B50" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C50" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" s="30"/>
-      <c r="E50" s="16" t="s">
+      <c r="C50" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="27"/>
+      <c r="E50" s="14" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="24" t="s">
+      <c r="A51" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="B51" s="24" t="s">
+      <c r="B51" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C51" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" s="49"/>
-      <c r="E51" s="50" t="s">
+      <c r="C51" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="38"/>
+      <c r="E51" s="39" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="24" t="s">
+      <c r="A52" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="B52" s="24" t="s">
+      <c r="B52" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C52" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D52" s="49"/>
-      <c r="E52" s="51" t="s">
+      <c r="C52" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="38"/>
+      <c r="E52" s="40" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="38" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="36" t="s">
+    <row r="53" spans="1:5" s="32" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="B53" s="36" t="s">
+      <c r="B53" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C53" s="36" t="s">
+      <c r="C53" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="D53" s="36"/>
-      <c r="E53" s="37" t="s">
+      <c r="D53" s="30"/>
+      <c r="E53" s="31" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="38" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="39" t="s">
+    <row r="54" spans="1:5" s="32" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="33" t="s">
         <v>209</v>
       </c>
-      <c r="B54" s="39" t="s">
+      <c r="B54" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="C54" s="39" t="s">
+      <c r="C54" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="D54" s="39"/>
-      <c r="E54" s="37" t="s">
+      <c r="D54" s="33"/>
+      <c r="E54" s="31" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="27"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
+      <c r="A55" s="25"/>
+      <c r="B55" s="24"/>
+      <c r="C55" s="24"/>
     </row>
     <row r="56" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="31" t="s">
+      <c r="A56" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="B56" s="32"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="15" t="s">
+      <c r="B56" s="57"/>
+      <c r="C56" s="57"/>
+      <c r="D56" s="58"/>
+      <c r="E56" s="13" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="30" t="s">
+      <c r="A57" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="B57" s="24" t="s">
+      <c r="B57" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="C57" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D57" s="30" t="s">
+      <c r="C57" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E57" s="25" t="s">
+      <c r="E57" s="23" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="30" t="s">
+      <c r="A58" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="B58" s="19" t="s">
+      <c r="B58" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C58" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D58" s="30"/>
-      <c r="E58" s="25" t="s">
+      <c r="C58" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" s="27"/>
+      <c r="E58" s="23" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="30" t="s">
+      <c r="A59" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="B59" s="30" t="s">
+      <c r="B59" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C59" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D59" s="30"/>
-      <c r="E59" s="25" t="s">
+      <c r="C59" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" s="27"/>
+      <c r="E59" s="23" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="30" t="s">
+      <c r="A60" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B60" s="24" t="s">
+      <c r="B60" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="C60" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D60" s="30" t="s">
+      <c r="C60" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="E60" s="25" t="s">
+      <c r="E60" s="23" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="27"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="26"/>
+      <c r="A61" s="25"/>
+      <c r="B61" s="24"/>
+      <c r="C61" s="24"/>
     </row>
     <row r="62" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="27"/>
-      <c r="B62" s="26"/>
-      <c r="C62" s="26"/>
+      <c r="A62" s="25"/>
+      <c r="B62" s="24"/>
+      <c r="C62" s="24"/>
     </row>
     <row r="63" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="29" t="s">
+      <c r="A63" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="B63" s="29"/>
-      <c r="C63" s="29"/>
-      <c r="D63" s="29"/>
-      <c r="E63" s="15" t="s">
+      <c r="B63" s="59"/>
+      <c r="C63" s="59"/>
+      <c r="D63" s="59"/>
+      <c r="E63" s="13" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="30" t="s">
+      <c r="A64" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B64" s="24" t="s">
+      <c r="B64" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="C64" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D64" s="24" t="s">
+      <c r="C64" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E64" s="52" t="s">
+      <c r="E64" s="41" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="30" t="s">
+      <c r="A65" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B65" s="30" t="s">
+      <c r="B65" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C65" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D65" s="30"/>
-      <c r="E65" s="52" t="s">
+      <c r="C65" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" s="27"/>
+      <c r="E65" s="41" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="66" spans="1:10" s="21" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="19" t="s">
+    <row r="66" spans="1:10" s="19" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="B66" s="19" t="s">
+      <c r="B66" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="C66" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D66" s="19"/>
-      <c r="E66" s="53" t="s">
+      <c r="C66" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" s="17"/>
+      <c r="E66" s="42" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="27"/>
-      <c r="B67" s="26"/>
-      <c r="C67" s="26"/>
+      <c r="A67" s="25"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="24"/>
     </row>
     <row r="69" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="14" t="s">
+      <c r="A69" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="B69" s="14"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="15" t="s">
+      <c r="B69" s="55"/>
+      <c r="C69" s="55"/>
+      <c r="D69" s="55"/>
+      <c r="E69" s="13" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="54" t="s">
+    <row r="70" spans="1:10" s="52" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="B70" s="24" t="s">
+      <c r="B70" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="C70" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="E70" s="52" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" s="19" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="C70" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="D70" s="55" t="s">
+      <c r="C71" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D71" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="E71" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="B72" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D72" s="22"/>
+      <c r="E72" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="F72" s="47"/>
+      <c r="G72" s="47"/>
+      <c r="H72" s="47"/>
+      <c r="I72" s="47"/>
+      <c r="J72" s="47"/>
+    </row>
+    <row r="73" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B73" s="69" t="s">
+        <v>106</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73" s="22"/>
+      <c r="E73" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="F73" s="47"/>
+      <c r="G73" s="47"/>
+      <c r="H73" s="47"/>
+      <c r="I73" s="47"/>
+      <c r="J73" s="47"/>
+    </row>
+    <row r="74" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="24"/>
+      <c r="B74" s="24"/>
+      <c r="C74" s="24"/>
+      <c r="D74" s="24"/>
+    </row>
+    <row r="75" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D75" s="35"/>
+    </row>
+    <row r="76" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="B76" s="64"/>
+      <c r="C76" s="64"/>
+      <c r="D76" s="64"/>
+      <c r="E76" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="B77" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="C77" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D77" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E70" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" s="21" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="20" t="s">
+      <c r="E77" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B71" s="19" t="s">
+      <c r="B78" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="C71" s="56" t="s">
-        <v>4</v>
-      </c>
-      <c r="D71" s="56" t="s">
-        <v>25</v>
-      </c>
-      <c r="E71" s="21" t="s">
+      <c r="C78" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78" s="22"/>
+      <c r="E78" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="24" t="s">
+    <row r="79" spans="1:10" s="19" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="B72" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C72" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D72" s="24"/>
-      <c r="E72" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="F72" s="58"/>
-      <c r="G72" s="58"/>
-      <c r="H72" s="58"/>
-      <c r="I72" s="58"/>
-      <c r="J72" s="58"/>
-    </row>
-    <row r="73" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="B73" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="C73" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D73" s="24"/>
-      <c r="E73" s="57" t="s">
-        <v>107</v>
-      </c>
-      <c r="F73" s="58"/>
-      <c r="G73" s="58"/>
-      <c r="H73" s="58"/>
-      <c r="I73" s="58"/>
-      <c r="J73" s="58"/>
-    </row>
-    <row r="74" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="26"/>
-      <c r="B74" s="26"/>
-      <c r="C74" s="26"/>
-      <c r="D74" s="26"/>
-    </row>
-    <row r="76" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="59" t="s">
-        <v>108</v>
-      </c>
-      <c r="B76" s="59"/>
-      <c r="C76" s="59"/>
-      <c r="D76" s="59"/>
-      <c r="E76" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="B77" s="24" t="s">
+      <c r="B79" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C79" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D79" s="17"/>
+      <c r="E79" s="42" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" s="48" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B80" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C80" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80" s="22"/>
+      <c r="E80" s="25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="81" spans="1:24" s="48" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B81" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81" s="22"/>
+      <c r="E81" s="48" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="82" spans="1:24" s="48" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B82" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="C82" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" s="22"/>
+      <c r="E82" s="48" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="83" spans="1:24" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="48"/>
+      <c r="B83" s="48"/>
+      <c r="C83" s="48"/>
+      <c r="D83" s="48"/>
+    </row>
+    <row r="84" spans="1:24" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="B84" s="59"/>
+      <c r="C84" s="59"/>
+      <c r="D84" s="59"/>
+      <c r="E84" s="34" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="85" spans="1:24" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="B85" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="C77" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D77" s="24" t="s">
+      <c r="C85" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E77" s="16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B78" s="24" t="s">
+      <c r="E85" s="23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="86" spans="1:24" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="B86" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C86" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D86" s="27"/>
+      <c r="E86" s="23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="88" spans="1:24" s="19" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="67" t="s">
+        <v>151</v>
+      </c>
+      <c r="B88" s="67"/>
+      <c r="C88" s="67"/>
+      <c r="D88" s="67"/>
+      <c r="E88" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="L88" s="14"/>
+      <c r="M88" s="14"/>
+      <c r="N88" s="14"/>
+    </row>
+    <row r="89" spans="1:24" s="19" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="B89" s="49" t="s">
         <v>145</v>
       </c>
-      <c r="C78" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D78" s="24"/>
-      <c r="E78" s="25" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" s="21" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="B79" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="C79" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D79" s="19"/>
-      <c r="E79" s="53" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" s="60" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B80" s="55" t="s">
-        <v>46</v>
-      </c>
-      <c r="C80" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="D80" s="24"/>
-      <c r="E80" s="27" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="81" spans="1:24" s="60" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="B81" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C81" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D81" s="24"/>
-      <c r="E81" s="60" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="82" spans="1:24" s="60" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="B82" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="C82" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="D82" s="24"/>
-      <c r="E82" s="60" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="83" spans="1:24" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="60"/>
-      <c r="B83" s="60"/>
-      <c r="C83" s="60"/>
-      <c r="D83" s="60"/>
-    </row>
-    <row r="84" spans="1:24" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="B84" s="29"/>
-      <c r="C84" s="29"/>
-      <c r="D84" s="29"/>
-      <c r="E84" s="40" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="85" spans="1:24" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="B85" s="24" t="s">
+      <c r="C89" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D89" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="E89" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="F89" s="14"/>
+      <c r="G89" s="14"/>
+      <c r="H89" s="14"/>
+      <c r="I89" s="14"/>
+      <c r="J89" s="14"/>
+      <c r="K89" s="14"/>
+      <c r="L89" s="14"/>
+      <c r="M89" s="14"/>
+      <c r="N89" s="14"/>
+      <c r="O89" s="14"/>
+      <c r="P89" s="14"/>
+      <c r="Q89" s="14"/>
+      <c r="R89" s="14"/>
+      <c r="S89" s="14"/>
+      <c r="T89" s="14"/>
+      <c r="U89" s="23"/>
+      <c r="V89" s="14"/>
+      <c r="W89" s="14"/>
+      <c r="X89" s="14"/>
+    </row>
+    <row r="90" spans="1:24" s="19" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="B90" s="49" t="s">
+        <v>154</v>
+      </c>
+      <c r="C90" s="50" t="s">
+        <v>163</v>
+      </c>
+      <c r="D90" s="49"/>
+      <c r="E90" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="14"/>
+      <c r="J90" s="14"/>
+      <c r="K90" s="14"/>
+      <c r="L90" s="14"/>
+      <c r="M90" s="14"/>
+      <c r="N90" s="14"/>
+      <c r="O90" s="14"/>
+      <c r="P90" s="14"/>
+      <c r="Q90" s="14"/>
+      <c r="R90" s="14"/>
+      <c r="S90" s="14"/>
+      <c r="T90" s="14"/>
+      <c r="U90" s="23"/>
+      <c r="V90" s="14"/>
+      <c r="W90" s="14"/>
+      <c r="X90" s="14"/>
+    </row>
+    <row r="91" spans="1:24" s="19" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="49" t="s">
+        <v>155</v>
+      </c>
+      <c r="B91" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C91" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D91" s="49"/>
+      <c r="E91" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="F91" s="14"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="14"/>
+      <c r="I91" s="14"/>
+      <c r="J91" s="14"/>
+      <c r="K91" s="14"/>
+      <c r="L91" s="14"/>
+      <c r="M91" s="14"/>
+      <c r="N91" s="14"/>
+      <c r="O91" s="14"/>
+      <c r="P91" s="14"/>
+      <c r="Q91" s="14"/>
+      <c r="R91" s="14"/>
+      <c r="S91" s="14"/>
+      <c r="T91" s="14"/>
+      <c r="U91" s="23"/>
+      <c r="V91" s="14"/>
+      <c r="W91" s="14"/>
+      <c r="X91" s="14"/>
+    </row>
+    <row r="92" spans="1:24" s="19" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="49" t="s">
+        <v>156</v>
+      </c>
+      <c r="B92" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="C92" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D92" s="49"/>
+      <c r="E92" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="F92" s="14"/>
+      <c r="G92" s="14"/>
+      <c r="H92" s="14"/>
+      <c r="I92" s="14"/>
+      <c r="J92" s="14"/>
+      <c r="K92" s="14"/>
+      <c r="L92" s="14"/>
+      <c r="M92" s="14"/>
+      <c r="N92" s="14"/>
+      <c r="O92" s="14"/>
+      <c r="P92" s="14"/>
+      <c r="Q92" s="14"/>
+      <c r="R92" s="14"/>
+      <c r="S92" s="14"/>
+      <c r="T92" s="14"/>
+      <c r="U92" s="23"/>
+      <c r="V92" s="14"/>
+      <c r="W92" s="14"/>
+      <c r="X92" s="14"/>
+    </row>
+    <row r="93" spans="1:24" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E93" s="23"/>
+      <c r="U93" s="23"/>
+    </row>
+    <row r="94" spans="1:24" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="67" t="s">
+        <v>166</v>
+      </c>
+      <c r="B94" s="67"/>
+      <c r="C94" s="67"/>
+      <c r="D94" s="67"/>
+      <c r="E94" s="13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="95" spans="1:24" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="49" t="s">
+        <v>168</v>
+      </c>
+      <c r="B95" s="49" t="s">
         <v>145</v>
       </c>
-      <c r="C85" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D85" s="30" t="s">
+      <c r="C95" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D95" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="E85" s="25" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="86" spans="1:24" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="B86" s="19" t="s">
+      <c r="E95" s="14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="96" spans="1:24" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="49" t="s">
+        <v>169</v>
+      </c>
+      <c r="B96" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="C86" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D86" s="30"/>
-      <c r="E86" s="25" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="88" spans="1:24" s="21" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="61" t="s">
-        <v>151</v>
-      </c>
-      <c r="B88" s="61"/>
-      <c r="C88" s="61"/>
-      <c r="D88" s="61"/>
-      <c r="E88" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="L88" s="16"/>
-      <c r="M88" s="16"/>
-      <c r="N88" s="16"/>
-    </row>
-    <row r="89" spans="1:24" s="21" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="62" t="s">
-        <v>152</v>
-      </c>
-      <c r="B89" s="62" t="s">
-        <v>145</v>
-      </c>
-      <c r="C89" s="62" t="s">
-        <v>4</v>
-      </c>
-      <c r="D89" s="62" t="s">
-        <v>5</v>
-      </c>
-      <c r="E89" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="F89" s="16"/>
-      <c r="G89" s="16"/>
-      <c r="H89" s="16"/>
-      <c r="I89" s="16"/>
-      <c r="J89" s="16"/>
-      <c r="K89" s="16"/>
-      <c r="L89" s="16"/>
-      <c r="M89" s="16"/>
-      <c r="N89" s="16"/>
-      <c r="O89" s="16"/>
-      <c r="P89" s="16"/>
-      <c r="Q89" s="16"/>
-      <c r="R89" s="16"/>
-      <c r="S89" s="16"/>
-      <c r="T89" s="16"/>
-      <c r="U89" s="25"/>
-      <c r="V89" s="16"/>
-      <c r="W89" s="16"/>
-      <c r="X89" s="16"/>
-    </row>
-    <row r="90" spans="1:24" s="21" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="62" t="s">
-        <v>153</v>
-      </c>
-      <c r="B90" s="62" t="s">
-        <v>154</v>
-      </c>
-      <c r="C90" s="63" t="s">
-        <v>163</v>
-      </c>
-      <c r="D90" s="62"/>
-      <c r="E90" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="F90" s="16"/>
-      <c r="G90" s="16"/>
-      <c r="H90" s="16"/>
-      <c r="I90" s="16"/>
-      <c r="J90" s="16"/>
-      <c r="K90" s="16"/>
-      <c r="L90" s="16"/>
-      <c r="M90" s="16"/>
-      <c r="N90" s="16"/>
-      <c r="O90" s="16"/>
-      <c r="P90" s="16"/>
-      <c r="Q90" s="16"/>
-      <c r="R90" s="16"/>
-      <c r="S90" s="16"/>
-      <c r="T90" s="16"/>
-      <c r="U90" s="25"/>
-      <c r="V90" s="16"/>
-      <c r="W90" s="16"/>
-      <c r="X90" s="16"/>
-    </row>
-    <row r="91" spans="1:24" s="21" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="62" t="s">
-        <v>155</v>
-      </c>
-      <c r="B91" s="62" t="s">
-        <v>18</v>
-      </c>
-      <c r="C91" s="62" t="s">
-        <v>4</v>
-      </c>
-      <c r="D91" s="62"/>
-      <c r="E91" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="F91" s="16"/>
-      <c r="G91" s="16"/>
-      <c r="H91" s="16"/>
-      <c r="I91" s="16"/>
-      <c r="J91" s="16"/>
-      <c r="K91" s="16"/>
-      <c r="L91" s="16"/>
-      <c r="M91" s="16"/>
-      <c r="N91" s="16"/>
-      <c r="O91" s="16"/>
-      <c r="P91" s="16"/>
-      <c r="Q91" s="16"/>
-      <c r="R91" s="16"/>
-      <c r="S91" s="16"/>
-      <c r="T91" s="16"/>
-      <c r="U91" s="25"/>
-      <c r="V91" s="16"/>
-      <c r="W91" s="16"/>
-      <c r="X91" s="16"/>
-    </row>
-    <row r="92" spans="1:24" s="21" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="62" t="s">
-        <v>156</v>
-      </c>
-      <c r="B92" s="62" t="s">
-        <v>157</v>
-      </c>
-      <c r="C92" s="62" t="s">
-        <v>4</v>
-      </c>
-      <c r="D92" s="62"/>
-      <c r="E92" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="F92" s="16"/>
-      <c r="G92" s="16"/>
-      <c r="H92" s="16"/>
-      <c r="I92" s="16"/>
-      <c r="J92" s="16"/>
-      <c r="K92" s="16"/>
-      <c r="L92" s="16"/>
-      <c r="M92" s="16"/>
-      <c r="N92" s="16"/>
-      <c r="O92" s="16"/>
-      <c r="P92" s="16"/>
-      <c r="Q92" s="16"/>
-      <c r="R92" s="16"/>
-      <c r="S92" s="16"/>
-      <c r="T92" s="16"/>
-      <c r="U92" s="25"/>
-      <c r="V92" s="16"/>
-      <c r="W92" s="16"/>
-      <c r="X92" s="16"/>
-    </row>
-    <row r="93" spans="1:24" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E93" s="25"/>
-      <c r="U93" s="25"/>
-    </row>
-    <row r="94" spans="1:24" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="61" t="s">
-        <v>166</v>
-      </c>
-      <c r="B94" s="61"/>
-      <c r="C94" s="61"/>
-      <c r="D94" s="61"/>
-      <c r="E94" s="15" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="95" spans="1:24" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="62" t="s">
-        <v>168</v>
-      </c>
-      <c r="B95" s="62" t="s">
-        <v>145</v>
-      </c>
-      <c r="C95" s="62" t="s">
-        <v>4</v>
-      </c>
-      <c r="D95" s="62" t="s">
-        <v>5</v>
-      </c>
-      <c r="E95" s="16" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="96" spans="1:24" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="62" t="s">
-        <v>169</v>
-      </c>
-      <c r="B96" s="62" t="s">
-        <v>157</v>
-      </c>
-      <c r="C96" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="D96" s="62"/>
-      <c r="E96" s="16" t="s">
+      <c r="C96" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D96" s="49"/>
+      <c r="E96" s="14" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="62" t="s">
+      <c r="A97" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="B97" s="62" t="str">
+      <c r="B97" s="49" t="str">
         <f>B64</f>
         <v>smallint</v>
       </c>
-      <c r="C97" s="62" t="s">
-        <v>4</v>
-      </c>
-      <c r="D97" s="62" t="s">
+      <c r="C97" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D97" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="E97" s="16" t="s">
+      <c r="E97" s="14" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="62" t="s">
+      <c r="A98" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="B98" s="62" t="str">
+      <c r="B98" s="49" t="str">
         <f>B57</f>
         <v>smallint</v>
       </c>
-      <c r="C98" s="62" t="s">
-        <v>4</v>
-      </c>
-      <c r="D98" s="62" t="s">
+      <c r="C98" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D98" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="E98" s="16" t="s">
+      <c r="E98" s="14" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="62" t="s">
+      <c r="A99" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="B99" s="62" t="s">
+      <c r="B99" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="C99" s="62" t="s">
-        <v>4</v>
-      </c>
-      <c r="D99" s="62"/>
-      <c r="E99" s="16" t="s">
+      <c r="C99" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D99" s="49"/>
+      <c r="E99" s="14" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="62" t="s">
+      <c r="A100" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="B100" s="62" t="s">
+      <c r="B100" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="C100" s="62"/>
-      <c r="D100" s="62"/>
-      <c r="E100" s="16" t="s">
+      <c r="C100" s="49"/>
+      <c r="D100" s="49"/>
+      <c r="E100" s="14" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="62" t="s">
+      <c r="A101" s="49" t="s">
         <v>172</v>
       </c>
-      <c r="B101" s="62" t="s">
+      <c r="B101" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="C101" s="62"/>
-      <c r="D101" s="62"/>
-      <c r="E101" s="16" t="s">
+      <c r="C101" s="49"/>
+      <c r="D101" s="49"/>
+      <c r="E101" s="14" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="61" t="s">
+      <c r="A103" s="67" t="s">
         <v>191</v>
       </c>
-      <c r="B103" s="61"/>
-      <c r="C103" s="61"/>
-      <c r="D103" s="61"/>
-      <c r="E103" s="15" t="s">
+      <c r="B103" s="67"/>
+      <c r="C103" s="67"/>
+      <c r="D103" s="67"/>
+      <c r="E103" s="13" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="62" t="s">
+      <c r="A104" s="49" t="s">
         <v>186</v>
       </c>
-      <c r="B104" s="62" t="s">
+      <c r="B104" s="49" t="s">
         <v>145</v>
       </c>
-      <c r="C104" s="62" t="s">
+      <c r="C104" s="49" t="s">
         <v>192</v>
       </c>
-      <c r="D104" s="62" t="s">
+      <c r="D104" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="E104" s="16" t="s">
+      <c r="E104" s="14" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="62" t="s">
+      <c r="A105" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="B105" s="62" t="s">
+      <c r="B105" s="49" t="s">
         <v>145</v>
       </c>
-      <c r="C105" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="D105" s="62" t="s">
+      <c r="C105" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D105" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="E105" s="21" t="s">
+      <c r="E105" s="19" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="62" t="s">
+      <c r="A106" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B106" s="62" t="s">
+      <c r="B106" s="49" t="s">
         <v>145</v>
       </c>
-      <c r="C106" s="62" t="s">
-        <v>4</v>
-      </c>
-      <c r="D106" s="62" t="s">
+      <c r="C106" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D106" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="E106" s="21" t="s">
+      <c r="E106" s="19" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="62" t="s">
+      <c r="A107" s="49" t="s">
         <v>207</v>
       </c>
-      <c r="B107" s="62" t="s">
+      <c r="B107" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="C107" s="62" t="s">
-        <v>4</v>
-      </c>
-      <c r="D107" s="62"/>
-      <c r="E107" s="16" t="s">
+      <c r="C107" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D107" s="49"/>
+      <c r="E107" s="14" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="62" t="s">
+      <c r="A108" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="B108" s="62" t="s">
+      <c r="B108" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C108" s="62" t="s">
-        <v>4</v>
-      </c>
-      <c r="D108" s="62"/>
-      <c r="E108" s="16" t="s">
+      <c r="C108" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D108" s="49"/>
+      <c r="E108" s="14" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="111" spans="1:5" s="66" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="64" t="s">
+    <row r="111" spans="1:5" s="52" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="62" t="s">
         <v>220</v>
       </c>
-      <c r="B111" s="64"/>
-      <c r="C111" s="64"/>
-      <c r="D111" s="64"/>
-      <c r="E111" s="65" t="s">
+      <c r="B111" s="62"/>
+      <c r="C111" s="62"/>
+      <c r="D111" s="62"/>
+      <c r="E111" s="51" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="112" spans="1:5" s="66" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="67" t="s">
+    <row r="112" spans="1:5" s="52" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="53" t="s">
         <v>221</v>
       </c>
-      <c r="B112" s="67" t="s">
+      <c r="B112" s="53" t="s">
         <v>145</v>
       </c>
-      <c r="C112" s="67" t="s">
-        <v>4</v>
-      </c>
-      <c r="D112" s="67" t="s">
+      <c r="C112" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="D112" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="E112" s="68" t="s">
+      <c r="E112" s="54" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="66" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="67" t="s">
+    <row r="113" spans="1:5" s="52" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="53" t="s">
         <v>118</v>
       </c>
-      <c r="B113" s="67" t="s">
+      <c r="B113" s="53" t="s">
         <v>157</v>
       </c>
-      <c r="C113" s="67" t="s">
-        <v>4</v>
-      </c>
-      <c r="D113" s="67"/>
-      <c r="E113" s="68" t="s">
+      <c r="C113" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="D113" s="53"/>
+      <c r="E113" s="54" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C121" s="43"/>
+      <c r="C121" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="D41:D42"/>
     <mergeCell ref="A111:D111"/>
     <mergeCell ref="E41:M42"/>
     <mergeCell ref="A84:D84"/>
@@ -3112,6 +3123,13 @@
     <mergeCell ref="A103:D103"/>
     <mergeCell ref="A94:D94"/>
     <mergeCell ref="A88:D88"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="D41:D42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3136,61 +3154,61 @@
       <c r="A1" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="68" t="s">
         <v>211</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="68" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="68" t="s">
         <v>215</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="68" t="s">
         <v>217</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="68" t="s">
         <v>219</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>